<commit_message>
Change how to get model (previouse one is compare the accuracy on dev set then test set
</commit_message>
<xml_diff>
--- a/data/Loi_ngu_phap.xlsx
+++ b/data/Loi_ngu_phap.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1.UIT\Nam 4\Hoc ky 2\Khai thac du lieu truyen thong xa hoi - IE403.K21\3. Implementing\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1.UIT\Nam 4\Hoc ky 2\Khai thac du lieu truyen thong xa hoi - IE403.K21\Nhom3-15520395-15520632-15520710-16520568\Source\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A963A5D-81C3-44C2-92C2-F72C1E0EF4A5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4D5101-00F0-4249-9F1C-874D5A2FDB96}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="196" xr2:uid="{E856D791-C2D0-4EA8-A531-FA55C3E03745}"/>
   </bookViews>
@@ -3912,68 +3912,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -4285,7 +4224,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{843B7CBE-AC69-4CC0-8B63-A7A77F45C9C1}">
   <dimension ref="A1:UW24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="CG1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="CM1" sqref="CM1:CM1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
@@ -4565,7 +4506,7 @@
         <v>307</v>
       </c>
       <c r="CM1" t="s">
-        <v>84</v>
+        <v>10</v>
       </c>
       <c r="CN1" t="s">
         <v>504</v>
@@ -8055,7 +7996,7 @@
     </row>
     <row r="9" spans="1:569" x14ac:dyDescent="0.4">
       <c r="CM9" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="JH9" t="s">
         <v>92</v>

</xml_diff>